<commit_message>
Move bike lane miles to sandag inputs, update the draft scenario check off
</commit_message>
<xml_diff>
--- a/off_model_calculators/sandag_inputs/Draft Scenario off model.xlsx
+++ b/off_model_calculators/sandag_inputs/Draft Scenario off model.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\RES\TransModel\2019RTP\off_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helseljw\OneDrive - WSP O365\SANDAG\RTP 2019\off_model_calculators\sandag_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2310EED8-4544-4C7A-9B7D-0AEA063DA662}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="10095" xr2:uid="{806C866B-30D3-4797-B854-9FF3A4CB2B6E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19176" windowHeight="10092"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="091818" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,8 +23,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>John Helsel</author>
+  </authors>
+  <commentList>
+    <comment ref="F8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>John Helsel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+waiting for update from Ying on Community-Based Coverage Areas tab</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
   <si>
     <t>No Build</t>
   </si>
@@ -94,13 +127,19 @@
   </si>
   <si>
     <t>2050F</t>
+  </si>
+  <si>
+    <t>*This color means the sheet has been completed.</t>
+  </si>
+  <si>
+    <t>*This color means the year cannot be completed (2050 data has not been provided)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,19 +155,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -148,6 +194,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -396,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -413,90 +471,66 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -515,10 +549,50 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -834,237 +908,253 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3601BE-EB61-4F84-8DF3-25B345557F11}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="40" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="42" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="43"/>
+      <c r="I1" s="33"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="37">
         <v>2035</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="38">
         <v>2050</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="17" t="s">
+      <c r="D3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="46" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="17" t="s">
+      <c r="B4" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="46" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="17" t="s">
+      <c r="B5" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="46" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
+      <c r="B6" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14" t="s">
+      <c r="B7" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="20"/>
+      <c r="G7" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="15"/>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
+      <c r="B8" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="33" t="s">
+      <c r="B9" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="34"/>
-      <c r="I9" s="35"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1074,5 +1164,6 @@
     <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update progress for Draft Scenario off model.xlsx
</commit_message>
<xml_diff>
--- a/off_model_calculators/sandag_inputs/Draft Scenario off model.xlsx
+++ b/off_model_calculators/sandag_inputs/Draft Scenario off model.xlsx
@@ -23,40 +23,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>John Helsel</author>
-  </authors>
-  <commentList>
-    <comment ref="F8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>John Helsel:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-waiting for update from Ying on Community-Based Coverage Areas tab</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
   <si>
@@ -139,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,21 +121,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +159,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -454,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -506,9 +465,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -531,31 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -593,6 +525,36 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -908,11 +870,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -923,31 +885,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="28" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30" t="s">
+      <c r="E1" s="44"/>
+      <c r="F1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32" t="s">
+      <c r="G1" s="46"/>
+      <c r="H1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="33"/>
+      <c r="I1" s="48"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="37">
+      <c r="B2" s="28">
         <v>2035</v>
       </c>
-      <c r="C2" s="38">
+      <c r="C2" s="29">
         <v>2050</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -973,28 +935,28 @@
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="34" t="s">
+      <c r="B3" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="37" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="37" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I3" s="37" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1002,28 +964,28 @@
       <c r="A4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="46" t="s">
+      <c r="B4" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="37" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1031,28 +993,28 @@
       <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="46" t="s">
+      <c r="B5" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="37" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1060,10 +1022,10 @@
       <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="34" t="s">
+      <c r="B6" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="9"/>
@@ -1071,7 +1033,7 @@
       <c r="F6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="46" t="s">
+      <c r="G6" s="37" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="12"/>
@@ -1081,18 +1043,18 @@
       <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="34" t="s">
+      <c r="B7" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="47" t="s">
+      <c r="G7" s="38" t="s">
         <v>6</v>
       </c>
       <c r="H7" s="12"/>
@@ -1102,57 +1064,57 @@
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="34" t="s">
+      <c r="B8" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="27" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="18"/>
-      <c r="F8" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="21"/>
+      <c r="F8" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="49" t="s">
+      <c r="B9" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="27"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="26"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="43" t="s">
+      <c r="B11" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="34" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="45" t="s">
+      <c r="B12" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="36" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1164,6 +1126,5 @@
     <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>